<commit_message>
Q-2 sent to students in pak - shoaib and hassan
</commit_message>
<xml_diff>
--- a/5_Homeworks/6_Teachning_New/Assignments.xlsx
+++ b/5_Homeworks/6_Teachning_New/Assignments.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\Python\5_Homeworks\6_Teachning_New\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784FC24C-8605-41A6-9387-7A29FC72233B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6EBB97-301C-4B46-BA8A-DB25BD5BCB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7193D43C-E26D-4186-AE3A-0B9DCF8DA726}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Date:</t>
   </si>
@@ -66,13 +67,529 @@
   </si>
   <si>
     <t>Python Programming - Coaching</t>
+  </si>
+  <si>
+    <t>2022-10-19</t>
+  </si>
+  <si>
+    <t>Q-2:</t>
+  </si>
+  <si>
+    <t>Computes income taxes, using a simplified tax schedule ?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006CB7"/>
+        <rFont val="StempelGaramond-Roman"/>
+      </rPr>
+      <t>Initialize constant variables for the tax rates and rate limits.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">6 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t xml:space="preserve">RATE1 = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF6FBF55"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>0.10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">7 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t xml:space="preserve">RATE2 = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF6FBF55"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>0.25</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">8 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t xml:space="preserve">RATE1_SINGLE_LIMIT = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF6FBF55"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>32000.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">9 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t xml:space="preserve">RATE1_MARRIED_LIMIT = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF6FBF55"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>64000.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">11 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF006CB7"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t xml:space="preserve"># </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006CB7"/>
+        <rFont val="StempelGaramond-Roman"/>
+      </rPr>
+      <t>Read income and marital status.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">12 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t xml:space="preserve">income = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDA511F"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>float</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDA511F"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF1DACAE"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>"Please enter your income: "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">13 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t xml:space="preserve">maritalStatus = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFDA511F"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF1DACAE"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>"Please enter s for single, m for married: "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">15 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF006CB7"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t xml:space="preserve"># </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF006CB7"/>
+        <rFont val="StempelGaramond-Roman"/>
+      </rPr>
+      <t>Compute taxes due.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">16 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t xml:space="preserve">tax1 = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF6FBF55"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>0.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">17 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t xml:space="preserve">tax2 = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF6FBF55"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>0.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">19 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFC82354"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t xml:space="preserve">if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t xml:space="preserve">maritalStatus == </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF1DACAE"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t xml:space="preserve">"s" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">20 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFC82354"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t xml:space="preserve">if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>income &lt;= RATE1_SINGLE_LIMIT :</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">21 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>tax1 = RATE1 * income</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">22 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFC82354"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t xml:space="preserve">else </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">23 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>tax1 = RATE1 * RATE1_SINGLE_LIMIT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">24 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>tax2 = RATE2 * (income - RATE1_SINGLE_LIMIT)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">25 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFC82354"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t xml:space="preserve">else </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">26 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFC82354"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t xml:space="preserve">if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>income &lt;= RATE1_MARRIED_LIMIT :</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">27 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>tax1 = RATE1 * income</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">28 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFC82354"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t xml:space="preserve">else </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">29 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>tax1 = RATE1 * RATE1_MARRIED_LIMIT</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">30 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF242021"/>
+        <rFont val="LucidaSansTypewriter"/>
+      </rPr>
+      <t>tax2 = RATE2 * (income - RATE1_MARRIED_LIMIT)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -129,6 +646,47 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF006CB7"/>
+      <name val="LucidaSansTypewriter"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006CB7"/>
+      <name val="StempelGaramond-Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF006CB7"/>
+      <name val="LucidaSans-Bold"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF242021"/>
+      <name val="LucidaSansTypewriter"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF6FBF55"/>
+      <name val="LucidaSansTypewriter"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFDA511F"/>
+      <name val="LucidaSansTypewriter"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF1DACAE"/>
+      <name val="LucidaSansTypewriter"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFC82354"/>
+      <name val="LucidaSansTypewriter"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -183,7 +741,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -201,12 +759,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -288,6 +850,138 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>379271</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>27887</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152038</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58C83EFA-80C6-3A3F-08C2-8B4FFD2E1D86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5351321" y="2238374"/>
+          <a:ext cx="3306216" cy="1733189"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>171068</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>47555</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2578B745-3A78-7165-A787-945D1238EB89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1476375" y="2657475"/>
+          <a:ext cx="3057143" cy="561905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>171069</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>66611</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC3A312E-19A7-819E-77C8-3E1C0AC36A5F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1485900" y="3209925"/>
+          <a:ext cx="3047619" cy="514286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -595,7 +1289,7 @@
   <dimension ref="A2:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:C12"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -605,7 +1299,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="19.5">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="2"/>
@@ -627,10 +1321,10 @@
       </c>
     </row>
     <row r="6" spans="1:18" s="1" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="16" t="s">
         <v>3</v>
       </c>
     </row>
@@ -665,7 +1359,7 @@
       <c r="B10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="6"/>
@@ -687,7 +1381,7 @@
     <row r="11" spans="1:18">
       <c r="A11" s="3"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="6"/>
@@ -709,7 +1403,7 @@
     <row r="12" spans="1:18">
       <c r="A12" s="3"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="6"/>
@@ -730,7 +1424,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="3"/>
-      <c r="C13" s="13"/>
+      <c r="C13" s="12"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -747,110 +1441,51 @@
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18">
-      <c r="A14" s="3"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-    </row>
-    <row r="15" spans="1:18">
-      <c r="A15" s="3"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
-    </row>
-    <row r="16" spans="1:18">
+    <row r="14" spans="1:18" s="1" customFormat="1">
+      <c r="B14" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" s="1" customFormat="1" ht="16.5" customHeight="1">
+      <c r="B15" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="14.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-    </row>
-    <row r="17" spans="1:18">
+      <c r="B16" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="10"/>
+    </row>
+    <row r="17" spans="1:18" ht="14.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="3"/>
       <c r="B18" s="1"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="3"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="5"/>
+      <c r="C19" s="12"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -867,6 +1502,46 @@
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
     </row>
+    <row r="20" spans="1:18">
+      <c r="A20" s="3"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21" s="3"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+    </row>
     <row r="23" spans="1:18">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -877,4 +1552,254 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F19AFE8-52F4-49AE-89E2-BFDC80831339}">
+  <dimension ref="E8:F33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8:F33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="8" spans="5:6">
+      <c r="E8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="str">
+        <f>RIGHT(E8,LEN(E8)-1)</f>
+        <v xml:space="preserve"> Initialize constant variables for the tax rates and rate limits.</v>
+      </c>
+    </row>
+    <row r="9" spans="5:6">
+      <c r="E9" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" ref="F9:F33" si="0">RIGHT(E9,LEN(E9)-1)</f>
+        <v xml:space="preserve"> RATE1 = 0.10</v>
+      </c>
+    </row>
+    <row r="10" spans="5:6">
+      <c r="E10" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> RATE2 = 0.25</v>
+      </c>
+    </row>
+    <row r="11" spans="5:6">
+      <c r="E11" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> RATE1_SINGLE_LIMIT = 32000.0</v>
+      </c>
+    </row>
+    <row r="12" spans="5:6">
+      <c r="E12" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> RATE1_MARRIED_LIMIT = 64000.0</v>
+      </c>
+    </row>
+    <row r="13" spans="5:6">
+      <c r="E13" s="15">
+        <v>10</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="5:6">
+      <c r="E14" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="str">
+        <f>RIGHT(E14,LEN(E14)-2)</f>
+        <v xml:space="preserve"> # Read income and marital status.</v>
+      </c>
+    </row>
+    <row r="15" spans="5:6">
+      <c r="E15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" ref="F15:F33" si="1">RIGHT(E15,LEN(E15)-2)</f>
+        <v xml:space="preserve"> income = float(input("Please enter your income: "))</v>
+      </c>
+    </row>
+    <row r="16" spans="5:6">
+      <c r="E16" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> maritalStatus = input("Please enter s for single, m for married: ")</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6">
+      <c r="E17" s="15">
+        <v>14</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="5:6">
+      <c r="E18" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> # Compute taxes due.</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6">
+      <c r="E19" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> tax1 = 0.0</v>
+      </c>
+    </row>
+    <row r="20" spans="5:6">
+      <c r="E20" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> tax2 = 0.0</v>
+      </c>
+    </row>
+    <row r="21" spans="5:6">
+      <c r="E21" s="15">
+        <v>18</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="5:6">
+      <c r="E22" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> if maritalStatus == "s" :</v>
+      </c>
+    </row>
+    <row r="23" spans="5:6">
+      <c r="E23" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> if income &lt;= RATE1_SINGLE_LIMIT :</v>
+      </c>
+    </row>
+    <row r="24" spans="5:6">
+      <c r="E24" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> tax1 = RATE1 * income</v>
+      </c>
+    </row>
+    <row r="25" spans="5:6">
+      <c r="E25" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> else :</v>
+      </c>
+    </row>
+    <row r="26" spans="5:6">
+      <c r="E26" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> tax1 = RATE1 * RATE1_SINGLE_LIMIT</v>
+      </c>
+    </row>
+    <row r="27" spans="5:6">
+      <c r="E27" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> tax2 = RATE2 * (income - RATE1_SINGLE_LIMIT)</v>
+      </c>
+    </row>
+    <row r="28" spans="5:6">
+      <c r="E28" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> else :</v>
+      </c>
+    </row>
+    <row r="29" spans="5:6">
+      <c r="E29" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> if income &lt;= RATE1_MARRIED_LIMIT :</v>
+      </c>
+    </row>
+    <row r="30" spans="5:6">
+      <c r="E30" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> tax1 = RATE1 * income</v>
+      </c>
+    </row>
+    <row r="31" spans="5:6">
+      <c r="E31" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> else :</v>
+      </c>
+    </row>
+    <row r="32" spans="5:6">
+      <c r="E32" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> tax1 = RATE1 * RATE1_MARRIED_LIMIT</v>
+      </c>
+    </row>
+    <row r="33" spans="5:6">
+      <c r="E33" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> tax2 = RATE2 * (income - RATE1_MARRIED_LIMIT)</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Assignment-3 sent - comparison using booleans
</commit_message>
<xml_diff>
--- a/5_Homeworks/6_Teachning_New/Assignments.xlsx
+++ b/5_Homeworks/6_Teachning_New/Assignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\Python\5_Homeworks\6_Teachning_New\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6EBB97-301C-4B46-BA8A-DB25BD5BCB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DE75DE-AB7E-44E6-8C11-965486D43AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7193D43C-E26D-4186-AE3A-0B9DCF8DA726}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>Date:</t>
   </si>
@@ -583,6 +583,15 @@
       </rPr>
       <t>tax2 = RATE2 * (income - RATE1_MARRIED_LIMIT)</t>
     </r>
+  </si>
+  <si>
+    <t>2022-10-20</t>
+  </si>
+  <si>
+    <t>Q-3:</t>
+  </si>
+  <si>
+    <t>Compare the numbers in Python using boolean expressions?</t>
   </si>
 </sst>
 </file>
@@ -864,8 +873,8 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>27887</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>152038</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>37738</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -978,6 +987,94 @@
         <a:xfrm>
           <a:off x="1485900" y="3209925"/>
           <a:ext cx="3047619" cy="514286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>94876</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>161839</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EB148B3-0450-550D-72A0-7EAF4D04CACA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1466850" y="4533900"/>
+          <a:ext cx="2990476" cy="685714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>132974</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>95143</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E9182D6-E3AD-2596-216D-E502A7A6CA7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1485900" y="5267325"/>
+          <a:ext cx="3009524" cy="857143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1286,10 +1383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73071862-74E6-42A1-A162-368129F9B992}">
-  <dimension ref="A2:R23"/>
+  <dimension ref="A2:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1320,7 +1417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="1" customFormat="1" ht="16.5" customHeight="1">
+    <row r="6" spans="1:18" s="1" customFormat="1">
       <c r="B6" s="11" t="s">
         <v>2</v>
       </c>
@@ -1449,7 +1546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" s="1" customFormat="1" ht="16.5" customHeight="1">
+    <row r="15" spans="1:18" s="1" customFormat="1">
       <c r="B15" s="11" t="s">
         <v>11</v>
       </c>
@@ -1545,6 +1642,111 @@
     <row r="23" spans="1:18">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
+    </row>
+    <row r="26" spans="1:18" s="1" customFormat="1">
+      <c r="B26" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" s="1" customFormat="1">
+      <c r="B27" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="14.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="10"/>
+    </row>
+    <row r="29" spans="1:18" ht="14.25">
+      <c r="A29" s="3"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="A30" s="3"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="5"/>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31" s="3"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" s="3"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="6"/>
+      <c r="R32" s="6"/>
+    </row>
+    <row r="33" spans="1:18">
+      <c r="A33" s="3"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="6"/>
+    </row>
+    <row r="35" spans="1:18">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1578,7 +1780,7 @@
         <v>14</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" ref="F9:F33" si="0">RIGHT(E9,LEN(E9)-1)</f>
+        <f t="shared" ref="F9:F13" si="0">RIGHT(E9,LEN(E9)-1)</f>
         <v xml:space="preserve"> RATE1 = 0.10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New python assignment for students sent
</commit_message>
<xml_diff>
--- a/5_Homeworks/6_Teachning_New/Assignments.xlsx
+++ b/5_Homeworks/6_Teachning_New/Assignments.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\Python\5_Homeworks\6_Teachning_New\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DE75DE-AB7E-44E6-8C11-965486D43AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7F8E17-8BE5-4BCD-9472-14B1300F25AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7193D43C-E26D-4186-AE3A-0B9DCF8DA726}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Quiz" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>Date:</t>
   </si>
@@ -592,6 +592,15 @@
   </si>
   <si>
     <t>Compare the numbers in Python using boolean expressions?</t>
+  </si>
+  <si>
+    <t>2022-10-22</t>
+  </si>
+  <si>
+    <t>Q-4:</t>
+  </si>
+  <si>
+    <t>Use various string functions to carry out string operations ?</t>
   </si>
 </sst>
 </file>
@@ -750,14 +759,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -806,13 +812,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -867,13 +873,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>379271</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>27887</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>37738</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -911,13 +917,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>171068</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>47555</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -955,13 +961,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>171069</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>66611</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -999,13 +1005,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>94876</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>161839</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1043,13 +1049,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>132974</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>95143</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1075,6 +1081,50 @@
         <a:xfrm>
           <a:off x="1485900" y="5267325"/>
           <a:ext cx="3009524" cy="857143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>589962</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>37994</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6568E821-FF15-F29F-73EC-80832A9B8237}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1466850" y="5867400"/>
+          <a:ext cx="4704762" cy="847619"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1383,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73071862-74E6-42A1-A162-368129F9B992}">
-  <dimension ref="A2:R35"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:C27"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1395,358 +1445,366 @@
     <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" ht="19.5">
-      <c r="B2" s="13" t="s">
+    <row r="1" spans="1:18" ht="19.5">
+      <c r="B1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:18" s="3" customFormat="1">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:18" s="1" customFormat="1">
-      <c r="B5" s="8" t="s">
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:18" s="1" customFormat="1">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="1" customFormat="1">
-      <c r="B6" s="11" t="s">
+    <row r="3" spans="1:18" s="1" customFormat="1">
+      <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="14.25">
+    <row r="4" spans="1:18" ht="14.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9"/>
+    </row>
+    <row r="5" spans="1:18" ht="14.25">
+      <c r="A5" s="3"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="3"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="3"/>
-      <c r="B7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="10"/>
-    </row>
-    <row r="8" spans="1:18" ht="14.25">
+      <c r="B7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" s="3"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="3"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="5"/>
+      <c r="C9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="3"/>
-      <c r="B10" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-    </row>
-    <row r="11" spans="1:18">
-      <c r="A11" s="3"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-    </row>
-    <row r="12" spans="1:18">
-      <c r="A12" s="3"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-    </row>
-    <row r="13" spans="1:18">
+      <c r="C10" s="11"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+    </row>
+    <row r="11" spans="1:18" s="1" customFormat="1">
+      <c r="B11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" s="1" customFormat="1">
+      <c r="B12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="14.25">
       <c r="A13" s="3"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-    </row>
-    <row r="14" spans="1:18" s="1" customFormat="1">
-      <c r="B14" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" s="1" customFormat="1">
-      <c r="B15" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="14.25">
+      <c r="B13" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" spans="1:18" ht="14.25">
+      <c r="A14" s="3"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="3"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" s="3"/>
-      <c r="B16" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="10"/>
-    </row>
-    <row r="17" spans="1:18" ht="14.25">
+      <c r="C16" s="11"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17" s="3"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="3"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="1:18">
-      <c r="A19" s="3"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
     </row>
     <row r="20" spans="1:18">
-      <c r="A20" s="3"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-    </row>
-    <row r="21" spans="1:18">
-      <c r="A21" s="3"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-    </row>
-    <row r="23" spans="1:18">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="26" spans="1:18" s="1" customFormat="1">
-      <c r="B26" s="8" t="s">
+      <c r="C20" s="1"/>
+    </row>
+    <row r="22" spans="1:18" s="1" customFormat="1">
+      <c r="B22" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:18" s="1" customFormat="1">
-      <c r="B27" s="11" t="s">
+    <row r="23" spans="1:18" s="1" customFormat="1">
+      <c r="B23" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C23" s="15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="14.25">
+    <row r="24" spans="1:18" ht="14.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" spans="1:18" ht="14.25">
+      <c r="A25" s="3"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26" s="3"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="A27" s="3"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28" s="3"/>
-      <c r="B28" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="10"/>
-    </row>
-    <row r="29" spans="1:18" ht="14.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+    </row>
+    <row r="29" spans="1:18">
       <c r="A29" s="3"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-    </row>
-    <row r="30" spans="1:18">
-      <c r="A30" s="3"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="5"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="3"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
-      <c r="P31" s="6"/>
-      <c r="Q31" s="6"/>
-      <c r="R31" s="6"/>
-    </row>
-    <row r="32" spans="1:18">
-      <c r="A32" s="3"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="6"/>
-      <c r="R32" s="6"/>
-    </row>
-    <row r="33" spans="1:18">
-      <c r="A33" s="3"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="6"/>
-    </row>
-    <row r="35" spans="1:18">
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="34" spans="2:3" s="1" customFormat="1">
+      <c r="B34" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" s="1" customFormat="1">
+      <c r="B35" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1767,7 +1825,7 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
     <row r="8" spans="5:6">
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>13</v>
       </c>
       <c r="F8" t="str">
@@ -1776,7 +1834,7 @@
       </c>
     </row>
     <row r="9" spans="5:6">
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="14" t="s">
         <v>14</v>
       </c>
       <c r="F9" t="str">
@@ -1785,7 +1843,7 @@
       </c>
     </row>
     <row r="10" spans="5:6">
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="14" t="s">
         <v>15</v>
       </c>
       <c r="F10" t="str">
@@ -1794,7 +1852,7 @@
       </c>
     </row>
     <row r="11" spans="5:6">
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="14" t="s">
         <v>16</v>
       </c>
       <c r="F11" t="str">
@@ -1803,7 +1861,7 @@
       </c>
     </row>
     <row r="12" spans="5:6">
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="14" t="s">
         <v>17</v>
       </c>
       <c r="F12" t="str">
@@ -1812,7 +1870,7 @@
       </c>
     </row>
     <row r="13" spans="5:6">
-      <c r="E13" s="15">
+      <c r="E13" s="14">
         <v>10</v>
       </c>
       <c r="F13" t="str">
@@ -1821,7 +1879,7 @@
       </c>
     </row>
     <row r="14" spans="5:6">
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="14" t="s">
         <v>18</v>
       </c>
       <c r="F14" t="str">
@@ -1830,7 +1888,7 @@
       </c>
     </row>
     <row r="15" spans="5:6">
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="14" t="s">
         <v>19</v>
       </c>
       <c r="F15" t="str">
@@ -1839,7 +1897,7 @@
       </c>
     </row>
     <row r="16" spans="5:6">
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="14" t="s">
         <v>20</v>
       </c>
       <c r="F16" t="str">
@@ -1848,7 +1906,7 @@
       </c>
     </row>
     <row r="17" spans="5:6">
-      <c r="E17" s="15">
+      <c r="E17" s="14">
         <v>14</v>
       </c>
       <c r="F17" t="str">
@@ -1857,7 +1915,7 @@
       </c>
     </row>
     <row r="18" spans="5:6">
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="14" t="s">
         <v>21</v>
       </c>
       <c r="F18" t="str">
@@ -1866,7 +1924,7 @@
       </c>
     </row>
     <row r="19" spans="5:6">
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="14" t="s">
         <v>22</v>
       </c>
       <c r="F19" t="str">
@@ -1875,7 +1933,7 @@
       </c>
     </row>
     <row r="20" spans="5:6">
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="14" t="s">
         <v>23</v>
       </c>
       <c r="F20" t="str">
@@ -1884,7 +1942,7 @@
       </c>
     </row>
     <row r="21" spans="5:6">
-      <c r="E21" s="15">
+      <c r="E21" s="14">
         <v>18</v>
       </c>
       <c r="F21" t="str">
@@ -1893,7 +1951,7 @@
       </c>
     </row>
     <row r="22" spans="5:6">
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="14" t="s">
         <v>24</v>
       </c>
       <c r="F22" t="str">
@@ -1902,7 +1960,7 @@
       </c>
     </row>
     <row r="23" spans="5:6">
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F23" t="str">
@@ -1911,7 +1969,7 @@
       </c>
     </row>
     <row r="24" spans="5:6">
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="14" t="s">
         <v>26</v>
       </c>
       <c r="F24" t="str">
@@ -1920,7 +1978,7 @@
       </c>
     </row>
     <row r="25" spans="5:6">
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="14" t="s">
         <v>27</v>
       </c>
       <c r="F25" t="str">
@@ -1929,7 +1987,7 @@
       </c>
     </row>
     <row r="26" spans="5:6">
-      <c r="E26" s="15" t="s">
+      <c r="E26" s="14" t="s">
         <v>28</v>
       </c>
       <c r="F26" t="str">
@@ -1938,7 +1996,7 @@
       </c>
     </row>
     <row r="27" spans="5:6">
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="14" t="s">
         <v>29</v>
       </c>
       <c r="F27" t="str">
@@ -1947,7 +2005,7 @@
       </c>
     </row>
     <row r="28" spans="5:6">
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="14" t="s">
         <v>30</v>
       </c>
       <c r="F28" t="str">
@@ -1956,7 +2014,7 @@
       </c>
     </row>
     <row r="29" spans="5:6">
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="14" t="s">
         <v>31</v>
       </c>
       <c r="F29" t="str">
@@ -1965,7 +2023,7 @@
       </c>
     </row>
     <row r="30" spans="5:6">
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="14" t="s">
         <v>32</v>
       </c>
       <c r="F30" t="str">
@@ -1974,7 +2032,7 @@
       </c>
     </row>
     <row r="31" spans="5:6">
-      <c r="E31" s="15" t="s">
+      <c r="E31" s="14" t="s">
         <v>33</v>
       </c>
       <c r="F31" t="str">
@@ -1983,7 +2041,7 @@
       </c>
     </row>
     <row r="32" spans="5:6">
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="14" t="s">
         <v>34</v>
       </c>
       <c r="F32" t="str">
@@ -1992,7 +2050,7 @@
       </c>
     </row>
     <row r="33" spans="5:6">
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="14" t="s">
         <v>35</v>
       </c>
       <c r="F33" t="str">

</xml_diff>

<commit_message>
List assignment sent to students
</commit_message>
<xml_diff>
--- a/5_Homeworks/6_Teachning_New/Assignments.xlsx
+++ b/5_Homeworks/6_Teachning_New/Assignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\Python\5_Homeworks\6_Teachning_New\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7F8E17-8BE5-4BCD-9472-14B1300F25AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D877D05-0BBA-4B16-B914-203E44B45797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7193D43C-E26D-4186-AE3A-0B9DCF8DA726}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t>Date:</t>
   </si>
@@ -601,6 +601,15 @@
   </si>
   <si>
     <t>Use various string functions to carry out string operations ?</t>
+  </si>
+  <si>
+    <t>2022-10-24</t>
+  </si>
+  <si>
+    <t>Q-5:</t>
+  </si>
+  <si>
+    <t>Take three separate lists of names, ages and birth-dates and combine them and print them as single list as per below format?</t>
   </si>
 </sst>
 </file>
@@ -1133,6 +1142,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95029</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>9402</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0DDFC87-C10E-63A8-2EB6-794091F47147}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1466850" y="7162800"/>
+          <a:ext cx="1771429" cy="980952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1433,10 +1486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73071862-74E6-42A1-A162-368129F9B992}">
-  <dimension ref="A1:R35"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43:C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1804,6 +1857,22 @@
       </c>
       <c r="C35" s="15" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" s="1" customFormat="1">
+      <c r="B42" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" s="1" customFormat="1">
+      <c r="B43" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excellent updates for students 1st func assignment
</commit_message>
<xml_diff>
--- a/5_Homeworks/6_Teachning_New/Assignments.xlsx
+++ b/5_Homeworks/6_Teachning_New/Assignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\Python\5_Homeworks\6_Teachning_New\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D877D05-0BBA-4B16-B914-203E44B45797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612AE2A0-B272-4489-86C0-6C5B38CC1B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7193D43C-E26D-4186-AE3A-0B9DCF8DA726}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Date:</t>
   </si>
@@ -610,6 +610,15 @@
   </si>
   <si>
     <t>Take three separate lists of names, ages and birth-dates and combine them and print them as single list as per below format?</t>
+  </si>
+  <si>
+    <t>2022-10-31</t>
+  </si>
+  <si>
+    <t>Q-6:</t>
+  </si>
+  <si>
+    <t>Write a program having two functions i.e. main() and cuberoot(). Main should run program and return cube of user input integer. Return 0 if input less than zero.</t>
   </si>
 </sst>
 </file>
@@ -661,13 +670,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color rgb="FF242021"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color rgb="FF7030A0"/>
       <name val="Arial"/>
@@ -713,6 +715,13 @@
       <sz val="8"/>
       <color rgb="FFC82354"/>
       <name val="LucidaSansTypewriter"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -787,10 +796,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1186,6 +1195,94 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>133200</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>152355</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67C52ED6-7D49-413E-2B02-F21ADA61C5F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1466850" y="8734425"/>
+          <a:ext cx="1200000" cy="361905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190344</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>57105</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57AD5302-CBEC-8458-52FE-D393790B73F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1476375" y="9124950"/>
+          <a:ext cx="1247619" cy="361905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1486,10 +1583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73071862-74E6-42A1-A162-368129F9B992}">
-  <dimension ref="A1:R43"/>
+  <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43:C43"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1873,6 +1970,22 @@
       </c>
       <c r="C43" s="15" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" s="1" customFormat="1">
+      <c r="B51" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" s="1" customFormat="1">
+      <c r="B52" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New work for students and assignments
</commit_message>
<xml_diff>
--- a/5_Homeworks/6_Teachning_New/Assignments.xlsx
+++ b/5_Homeworks/6_Teachning_New/Assignments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\Python\5_Homeworks\6_Teachning_New\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612AE2A0-B272-4489-86C0-6C5B38CC1B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A2D0C9-A0E8-43C3-9BFF-923DA18232AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7193D43C-E26D-4186-AE3A-0B9DCF8DA726}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
   <si>
     <t>Date:</t>
   </si>
@@ -619,6 +619,15 @@
   </si>
   <si>
     <t>Write a program having two functions i.e. main() and cuberoot(). Main should run program and return cube of user input integer. Return 0 if input less than zero.</t>
+  </si>
+  <si>
+    <t>2022-11-23</t>
+  </si>
+  <si>
+    <t>Q-7:</t>
+  </si>
+  <si>
+    <t>Write a program having two functions i.e. days_in_month(year, month) will return days for any year and any month. Use helper function leap_year(year) to check leap years.</t>
   </si>
 </sst>
 </file>
@@ -1283,6 +1292,94 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>56857</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>9443</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78B38151-78D9-4F92-D5DB-03EC0062B791}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1466850" y="10077450"/>
+          <a:ext cx="2342857" cy="657143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>495238</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>161864</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5ADB583A-F38A-D9CE-9F30-91EC12DB14F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1466850" y="10725150"/>
+          <a:ext cx="495238" cy="485714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1583,10 +1680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73071862-74E6-42A1-A162-368129F9B992}">
-  <dimension ref="A1:R52"/>
+  <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61:C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1986,6 +2083,22 @@
       </c>
       <c r="C52" s="15" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" s="1" customFormat="1">
+      <c r="B60" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" s="1" customFormat="1">
+      <c r="B61" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New quiz for students
</commit_message>
<xml_diff>
--- a/5_Homeworks/6_Teachning_New/Assignments.xlsx
+++ b/5_Homeworks/6_Teachning_New/Assignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\Python\5_Homeworks\6_Teachning_New\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A2D0C9-A0E8-43C3-9BFF-923DA18232AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3BBB4D-5DAD-4916-A0F8-BA3AC69604AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7193D43C-E26D-4186-AE3A-0B9DCF8DA726}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>Date:</t>
   </si>
@@ -628,6 +628,15 @@
   </si>
   <si>
     <t>Write a program having two functions i.e. days_in_month(year, month) will return days for any year and any month. Use helper function leap_year(year) to check leap years.</t>
+  </si>
+  <si>
+    <t>2022-12-06</t>
+  </si>
+  <si>
+    <t>Q-8:</t>
+  </si>
+  <si>
+    <t>Now use days_in_month(year, month) to calculate difference of two dates as def days_between(year1, month1, day1, year2, month2, day2) with below details;</t>
   </si>
 </sst>
 </file>
@@ -1380,6 +1389,138 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>580438</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>56880</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30CCEC38-1248-8B99-3C33-4CD9B9185673}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1466850" y="11696700"/>
+          <a:ext cx="4695238" cy="2161905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>609162</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>133258</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A16919E0-2FB8-01A9-A3B0-5AB4D7F988F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1466850" y="13849350"/>
+          <a:ext cx="3504762" cy="733333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>361543</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>142811</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C932EEF-8BCB-C582-9F27-9AD98B29ACD8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1466850" y="14563725"/>
+          <a:ext cx="3257143" cy="514286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1680,10 +1821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73071862-74E6-42A1-A162-368129F9B992}">
-  <dimension ref="A1:R61"/>
+  <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61:C61"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2099,6 +2240,22 @@
       </c>
       <c r="C61" s="15" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" s="1" customFormat="1">
+      <c r="B70" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" s="1" customFormat="1">
+      <c r="B71" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>